<commit_message>
cambios desde mac para seguir a windows
</commit_message>
<xml_diff>
--- a/peso-especifico.xlsx
+++ b/peso-especifico.xlsx
@@ -34,13 +34,13 @@
     <t>N</t>
   </si>
   <si>
-    <t>Chapa Negra SAE 1010</t>
+    <t>Negra</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>Chapa Galvanizada SAE 1010</t>
+    <t>Galvanizada</t>
   </si>
   <si>
     <t>I</t>
@@ -52,7 +52,7 @@
     <t>S</t>
   </si>
   <si>
-    <t>Chapa semilla de melón</t>
+    <t>Semilla de melón</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
     <col min="3" max="3" style="6" width="24.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -464,7 +464,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -475,7 +475,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -486,7 +486,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -497,7 +497,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>